<commit_message>
add GDPA & Menu
</commit_message>
<xml_diff>
--- a/Projects/CCZA_SAND/Data/Template.xlsx
+++ b/Projects/CCZA_SAND/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">sos_weights!$B$4:$AC$20</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="j" vbProcedure="false">list_of_entities!$B$4:$AB$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Trax" vbProcedure="false">list_of_entities!$B$4:$AB$4</definedName>
@@ -41,28 +41,34 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">list_of_entities!$B$4:$AB$142</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">list_of_entities!$B$4:$AB$142</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">list_of_entities!$B$4:$AB$142</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">list_of_entities!$B$4:$AB$142</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">sos_weights!$B$4:$AC$20</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0" vbProcedure="false">Pricing_targets!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -74,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4951" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4953" uniqueCount="410">
   <si>
     <t xml:space="preserve">Store types weight</t>
   </si>
@@ -1295,6 +1301,9 @@
   </si>
   <si>
     <t xml:space="preserve">Is Bonaqua available in the store?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Left to Right</t>
   </si>
   <si>
     <t xml:space="preserve">COCA-COLA, COCA COLA PLUS COFFEE, COKE ZERO, COKE LIGHT, COCA COLA NO SUGAR NO CAFFEINE, TAB, SPRITE, SPRITE ZERO, FANTA ORANGE, Fanta Mango, FANTA Pinapple, FANTA Grape, STONEY</t>
@@ -3303,9 +3312,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>389160</xdr:colOff>
+      <xdr:colOff>388800</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3315,7 +3324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10790280" cy="9131040"/>
+          <a:ext cx="10847160" cy="9130680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3356,13 +3365,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.3157894736842"/>
     <col collapsed="false" hidden="false" max="21" min="8" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="23" min="22" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.57085020242915"/>
@@ -4259,10 +4268,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.5587044534413"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.412955465587"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.9514170040486"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="18" min="10" style="0" width="8.57085020242915"/>
@@ -15434,11 +15443,11 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.2429149797571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.7044534412956"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.9878542510121"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.1336032388664"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.1740890688259"/>
     <col collapsed="false" hidden="false" max="10" min="7" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="17" min="12" style="0" width="8.57085020242915"/>
@@ -16965,7 +16974,7 @@
       <c r="AC21" s="167"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:AC20"/>
+  <autoFilter ref="B4:AC19"/>
   <mergeCells count="1">
     <mergeCell ref="L3:AC3"/>
   </mergeCells>
@@ -16995,8 +17004,8 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.9919028340081"/>
     <col collapsed="false" hidden="false" max="19" min="4" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.89068825910931"/>
@@ -18134,8 +18143,8 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.9878542510121"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.5222672064777"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="12" min="5" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="true" max="13" min="13" style="0" width="0"/>
@@ -20799,8 +20808,8 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.8785425101215"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.417004048583"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="22" min="5" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.57085020242915"/>
@@ -23471,11 +23480,11 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.4534412955466"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.8825910931174"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="92.7651821862348"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="93.6234817813765"/>
     <col collapsed="false" hidden="false" max="21" min="7" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="true" max="22" min="22" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="30" min="23" style="0" width="8.67611336032389"/>
@@ -26351,19 +26360,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.1578947368421"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.9109311740891"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -26392,6 +26401,9 @@
       <c r="H1" s="37" t="s">
         <v>56</v>
       </c>
+      <c r="I1" s="37" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="290" t="s">
@@ -26407,7 +26419,7 @@
         <v>214</v>
       </c>
       <c r="E2" s="291" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F2" s="290" t="s">
         <v>59</v>
@@ -26416,7 +26428,10 @@
         <v>60</v>
       </c>
       <c r="H2" s="290" t="s">
-        <v>408</v>
+        <v>409</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
flow changed to be always right to left
</commit_message>
<xml_diff>
--- a/Projects/CCZA_SAND/Data/Template.xlsx
+++ b/Projects/CCZA_SAND/Data/Template.xlsx
@@ -22,7 +22,7 @@
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">sos_weights!$B$4:$AC$20</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="j" vbProcedure="false">list_of_entities!$B$4:$AB$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Trax" vbProcedure="false">list_of_entities!$B$4:$AB$4</definedName>
@@ -42,33 +42,39 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">list_of_entities!$B$4:$AB$142</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">list_of_entities!$B$4:$AB$142</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">list_of_entities!$B$4:$AB$142</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">sos_weights!$B$4:$AC$20</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">list_of_entities!$B$4:$AB$142</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">sos_weights!$B$4:$AC$20</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">sos_weights!$B$4:$AC$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">sos_targets!$B$4:$U$19</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Pricing_weights!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0" vbProcedure="false">Pricing_targets!$B$4:$V$39</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Pricing_targets!$B$4:$V$43</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">survey_questions!$B$4:$AE$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -80,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4953" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4951" uniqueCount="409">
   <si>
     <t xml:space="preserve">Store types weight</t>
   </si>
@@ -1301,9 +1307,6 @@
   </si>
   <si>
     <t xml:space="preserve">Is Bonaqua available in the store?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is Left to Right</t>
   </si>
   <si>
     <t xml:space="preserve">COCA-COLA, COCA COLA PLUS COFFEE, COKE ZERO, COKE LIGHT, COCA COLA NO SUGAR NO CAFFEINE, TAB, SPRITE, SPRITE ZERO, FANTA ORANGE, Fanta Mango, FANTA Pinapple, FANTA Grape, STONEY</t>
@@ -3312,9 +3315,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>388800</xdr:colOff>
+      <xdr:colOff>388440</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>93600</xdr:rowOff>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3324,7 +3327,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10847160" cy="9130680"/>
+          <a:ext cx="10904040" cy="9130320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3365,13 +3368,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.5303643724696"/>
     <col collapsed="false" hidden="false" max="21" min="8" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="23" min="22" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.57085020242915"/>
@@ -4268,10 +4271,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9878542510121"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.9514170040486"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.5910931174089"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="18" min="10" style="0" width="8.57085020242915"/>
@@ -15443,11 +15446,11 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.1336032388664"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.3846153846154"/>
     <col collapsed="false" hidden="false" max="10" min="7" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="17" min="12" style="0" width="8.57085020242915"/>
@@ -16974,7 +16977,7 @@
       <c r="AC21" s="167"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:AC19"/>
+  <autoFilter ref="B4:AC20"/>
   <mergeCells count="1">
     <mergeCell ref="L3:AC3"/>
   </mergeCells>
@@ -17004,8 +17007,8 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.3117408906883"/>
     <col collapsed="false" hidden="false" max="19" min="4" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.89068825910931"/>
@@ -18143,8 +18146,8 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.5222672064777"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.0566801619433"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="12" min="5" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="true" max="13" min="13" style="0" width="0"/>
@@ -20808,8 +20811,8 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="22" min="5" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.57085020242915"/>
@@ -23480,11 +23483,11 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.8825910931174"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.3076923076923"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="93.6234817813765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="94.4777327935223"/>
     <col collapsed="false" hidden="false" max="21" min="7" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="true" max="22" min="22" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="30" min="23" style="0" width="8.67611336032389"/>
@@ -26360,19 +26363,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.9109311740891"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="86.6599190283401"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -26401,9 +26404,6 @@
       <c r="H1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>407</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="290" t="s">
@@ -26419,7 +26419,7 @@
         <v>214</v>
       </c>
       <c r="E2" s="291" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F2" s="290" t="s">
         <v>59</v>
@@ -26428,10 +26428,7 @@
         <v>60</v>
       </c>
       <c r="H2" s="290" t="s">
-        <v>409</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>349</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>